<commit_message>
Updated reference set based on close-to-final trees
</commit_message>
<xml_diff>
--- a/tabular/ifnl-side-data.xlsx
+++ b/tabular/ifnl-side-data.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11208"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/host/IFNL-Evolution/tabular/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{311CDEA4-E9DC-7845-A2C2-4A822955B82A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="740" yWindow="460" windowWidth="28060" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13980" yWindow="2580" windowWidth="28060" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="A+B" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -25,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1202" uniqueCount="404">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1203" uniqueCount="405">
   <si>
     <t>retroIFNL1a</t>
   </si>
@@ -1237,13 +1231,16 @@
   </si>
   <si>
     <t>NM_172138</t>
+  </si>
+  <si>
+    <t>Xenopus tropicalis</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1406,8 +1403,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="459">
+  <cellStyleXfs count="463">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1886,7 +1887,7 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="459">
+  <cellStyles count="463">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2116,6 +2117,8 @@
     <cellStyle name="Followed Hyperlink" xfId="454" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="456" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="458" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="460" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="462" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2345,6 +2348,8 @@
     <cellStyle name="Hyperlink" xfId="453" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="455" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="457" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="459" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="461" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2689,14 +2694,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="F36" sqref="A1:M110"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="A109" sqref="A109"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="16.1640625" customWidth="1"/>
     <col min="2" max="3" width="14.83203125" customWidth="1"/>
@@ -2764,7 +2769,9 @@
         <v>319</v>
       </c>
       <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
+      <c r="F2" s="11" t="s">
+        <v>404</v>
+      </c>
       <c r="G2" s="11"/>
       <c r="H2" s="11"/>
       <c r="I2" s="11"/>
@@ -5007,7 +5014,7 @@
       </c>
       <c r="M62" s="12"/>
     </row>
-    <row r="63" spans="1:13" s="6" customFormat="1">
+    <row r="63" spans="1:13" s="6" customFormat="1" ht="16">
       <c r="A63" s="12" t="s">
         <v>242</v>
       </c>
@@ -6766,7 +6773,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M110">
+  <sortState ref="A2:M110">
     <sortCondition ref="D2:D110"/>
     <sortCondition ref="I2:I110"/>
   </sortState>

</xml_diff>

<commit_message>
Created and validated the reference sequence set
</commit_message>
<xml_diff>
--- a/tabular/ifnl-side-data.xlsx
+++ b/tabular/ifnl-side-data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="13980" yWindow="2580" windowWidth="28060" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="620" yWindow="0" windowWidth="23480" windowHeight="20960" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="A+B" sheetId="2" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1203" uniqueCount="405">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1204" uniqueCount="411">
   <si>
     <t>retroIFNL1a</t>
   </si>
@@ -981,9 +981,6 @@
     <t>AMPH</t>
   </si>
   <si>
-    <t>MAMM</t>
-  </si>
-  <si>
     <t>MAMM4</t>
   </si>
   <si>
@@ -1234,6 +1231,27 @@
   </si>
   <si>
     <t>Xenopus tropicalis</t>
+  </si>
+  <si>
+    <t>IFNL-Amphibian</t>
+  </si>
+  <si>
+    <t>IFNL-Reptile</t>
+  </si>
+  <si>
+    <t>IFNL-Aves</t>
+  </si>
+  <si>
+    <t>IFNL-Mammal</t>
+  </si>
+  <si>
+    <t>IFNLa-Mammal</t>
+  </si>
+  <si>
+    <t>IFNLa-Reptile</t>
+  </si>
+  <si>
+    <t>Pelodiscus sinensis</t>
   </si>
 </sst>
 </file>
@@ -1403,8 +1421,32 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="463">
+  <cellStyleXfs count="487">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1887,7 +1929,7 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="463">
+  <cellStyles count="487">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2119,6 +2161,18 @@
     <cellStyle name="Followed Hyperlink" xfId="458" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="460" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="462" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="464" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="466" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="468" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="470" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="472" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="474" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="476" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="478" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="480" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="482" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="484" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="486" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2350,6 +2404,18 @@
     <cellStyle name="Hyperlink" xfId="457" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="459" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="461" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="463" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="465" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="467" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="469" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="471" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="473" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="475" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="477" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="479" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="481" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="483" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="485" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2697,8 +2763,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="A109" sqref="A109"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2730,7 +2796,7 @@
         <v>261</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>69</v>
@@ -2762,7 +2828,7 @@
         <v>311</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>319</v>
+        <v>404</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="11" t="s">
@@ -2770,7 +2836,7 @@
       </c>
       <c r="E2" s="11"/>
       <c r="F2" s="11" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="G2" s="11"/>
       <c r="H2" s="11"/>
@@ -2785,11 +2851,11 @@
         <v>312</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>322</v>
+        <v>409</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="8" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
@@ -2806,14 +2872,16 @@
         <v>313</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>323</v>
+        <v>405</v>
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="9" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
+      <c r="F4" s="9" t="s">
+        <v>410</v>
+      </c>
       <c r="G4" s="9"/>
       <c r="H4" s="9"/>
       <c r="I4" s="9"/>
@@ -2827,11 +2895,11 @@
         <v>314</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>323</v>
+        <v>405</v>
       </c>
       <c r="C5" s="9"/>
       <c r="D5" s="9" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E5" s="9"/>
       <c r="F5" s="9"/>
@@ -2848,11 +2916,11 @@
         <v>315</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>323</v>
+        <v>405</v>
       </c>
       <c r="C6" s="9"/>
       <c r="D6" s="9" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E6" s="9"/>
       <c r="F6" s="9"/>
@@ -2869,11 +2937,11 @@
         <v>316</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>324</v>
+        <v>406</v>
       </c>
       <c r="C7" s="10"/>
       <c r="D7" s="10" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="E7" s="10"/>
       <c r="F7" s="10"/>
@@ -2890,11 +2958,11 @@
         <v>317</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>324</v>
+        <v>406</v>
       </c>
       <c r="C8" s="10"/>
       <c r="D8" s="10" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="E8" s="10"/>
       <c r="F8" s="10"/>
@@ -2911,11 +2979,11 @@
         <v>318</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>324</v>
+        <v>406</v>
       </c>
       <c r="C9" s="10"/>
       <c r="D9" s="10" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="E9" s="10"/>
       <c r="F9" s="10"/>
@@ -2932,22 +3000,22 @@
         <v>250</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>320</v>
+        <v>407</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>320</v>
+        <v>328</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>115</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="H10" s="5" t="s">
         <v>115</v>
@@ -2973,22 +3041,22 @@
         <v>5</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>320</v>
+        <v>407</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>320</v>
+        <v>328</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>306</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="H11" s="5" t="s">
         <v>78</v>
@@ -3012,22 +3080,22 @@
         <v>251</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>320</v>
+        <v>407</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>320</v>
+        <v>328</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>306</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="H12" s="5" t="s">
         <v>78</v>
@@ -3051,22 +3119,22 @@
         <v>252</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>320</v>
+        <v>407</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>320</v>
+        <v>328</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>306</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="H13" s="5" t="s">
         <v>78</v>
@@ -3090,22 +3158,22 @@
         <v>4</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>320</v>
+        <v>407</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>132</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="H14" s="5" t="s">
         <v>74</v>
@@ -3129,22 +3197,22 @@
         <v>256</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>320</v>
+        <v>407</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>132</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="H15" s="5" t="s">
         <v>74</v>
@@ -3170,22 +3238,22 @@
         <v>224</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>320</v>
+        <v>407</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>129</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="H16" s="5" t="s">
         <v>74</v>
@@ -3209,22 +3277,22 @@
         <v>225</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>320</v>
+        <v>407</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>80</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="H17" s="5" t="s">
         <v>74</v>
@@ -3248,22 +3316,22 @@
         <v>226</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>320</v>
+        <v>407</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>80</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="H18" s="5" t="s">
         <v>74</v>
@@ -3287,22 +3355,22 @@
         <v>233</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>320</v>
+        <v>407</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E19" s="5" t="s">
         <v>113</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="H19" s="5" t="s">
         <v>115</v>
@@ -3328,22 +3396,22 @@
         <v>227</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>320</v>
+        <v>407</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>108</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="H20" s="5" t="s">
         <v>74</v>
@@ -3367,22 +3435,22 @@
         <v>253</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>320</v>
+        <v>407</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>142</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="H21" s="5" t="s">
         <v>78</v>
@@ -3406,22 +3474,22 @@
         <v>258</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>320</v>
+        <v>407</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E22" s="5" t="s">
         <v>111</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="H22" s="5" t="s">
         <v>74</v>
@@ -3445,22 +3513,22 @@
         <v>230</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>320</v>
+        <v>407</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E23" s="5" t="s">
         <v>147</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="H23" s="5" t="s">
         <v>74</v>
@@ -3484,22 +3552,22 @@
         <v>262</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>320</v>
+        <v>407</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E24" s="5" t="s">
         <v>77</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="H24" s="5" t="s">
         <v>78</v>
@@ -3523,13 +3591,13 @@
         <v>2</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>320</v>
+        <v>407</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E25" s="5" t="s">
         <v>77</v>
@@ -3538,7 +3606,7 @@
         <v>183</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="H25" s="5" t="s">
         <v>78</v>
@@ -3562,22 +3630,22 @@
         <v>254</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>320</v>
+        <v>407</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E26" s="5" t="s">
         <v>77</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="H26" s="5" t="s">
         <v>78</v>
@@ -3601,22 +3669,22 @@
         <v>221</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>320</v>
+        <v>407</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E27" s="5" t="s">
         <v>77</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="H27" s="5" t="s">
         <v>78</v>
@@ -3640,22 +3708,22 @@
         <v>222</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>320</v>
+        <v>407</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E28" s="5" t="s">
         <v>77</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="H28" s="5" t="s">
         <v>78</v>
@@ -3681,22 +3749,22 @@
         <v>304</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>320</v>
+        <v>407</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E29" s="5" t="s">
         <v>77</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="H29" s="5" t="s">
         <v>78</v>
@@ -3720,22 +3788,22 @@
         <v>3</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>320</v>
+        <v>407</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E30" s="5" t="s">
         <v>77</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="H30" s="5" t="s">
         <v>78</v>
@@ -3759,22 +3827,22 @@
         <v>223</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>320</v>
+        <v>407</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E31" s="5" t="s">
         <v>77</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="H31" s="5" t="s">
         <v>78</v>
@@ -3798,22 +3866,22 @@
         <v>255</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>320</v>
+        <v>407</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E32" s="5" t="s">
         <v>90</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="H32" s="5" t="s">
         <v>78</v>
@@ -3837,22 +3905,22 @@
         <v>218</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>320</v>
+        <v>407</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E33" s="5" t="s">
         <v>135</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="H33" s="5" t="s">
         <v>105</v>
@@ -3876,22 +3944,22 @@
         <v>219</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>320</v>
+        <v>407</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E34" s="5" t="s">
         <v>144</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="H34" s="5" t="s">
         <v>105</v>
@@ -3917,22 +3985,22 @@
         <v>257</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>320</v>
+        <v>407</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="G35" s="7" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="H35" s="7" t="s">
         <v>74</v>
@@ -3958,22 +4026,22 @@
         <v>72</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>320</v>
+        <v>407</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="G36" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H36" s="7" t="s">
         <v>74</v>
@@ -3997,22 +4065,22 @@
         <v>260</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>320</v>
+        <v>407</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="G37" s="7" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H37" s="7" t="s">
         <v>74</v>
@@ -4036,22 +4104,22 @@
         <v>228</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>320</v>
+        <v>407</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="G38" s="7" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="H38" s="7" t="s">
         <v>74</v>
@@ -4075,22 +4143,22 @@
         <v>229</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>320</v>
+        <v>407</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G39" s="7" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="H39" s="7" t="s">
         <v>74</v>
@@ -4114,22 +4182,22 @@
         <v>0</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>320</v>
+        <v>407</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="F40" s="7" t="s">
         <v>9</v>
       </c>
       <c r="G40" s="7" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="H40" s="7" t="s">
         <v>74</v>
@@ -4153,22 +4221,22 @@
         <v>231</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>320</v>
+        <v>407</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="G41" s="7" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="H41" s="7" t="s">
         <v>74</v>
@@ -4192,22 +4260,22 @@
         <v>220</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>320</v>
+        <v>407</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D42" s="7" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="F42" s="7" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="G42" s="7" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="H42" s="7" t="s">
         <v>105</v>
@@ -4233,22 +4301,22 @@
         <v>232</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>320</v>
+        <v>407</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="G43" s="7" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="H43" s="7" t="s">
         <v>74</v>
@@ -4272,22 +4340,22 @@
         <v>264</v>
       </c>
       <c r="B44" s="12" t="s">
-        <v>320</v>
+        <v>407</v>
       </c>
       <c r="C44" s="12" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D44" s="12" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E44" s="12" t="s">
         <v>132</v>
       </c>
       <c r="F44" s="12" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="G44" s="12" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="H44" s="12" t="s">
         <v>74</v>
@@ -4313,22 +4381,22 @@
         <v>243</v>
       </c>
       <c r="B45" s="12" t="s">
-        <v>320</v>
+        <v>407</v>
       </c>
       <c r="C45" s="12" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D45" s="12" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E45" s="12" t="s">
         <v>129</v>
       </c>
       <c r="F45" s="12" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="G45" s="12" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="H45" s="12" t="s">
         <v>74</v>
@@ -4352,22 +4420,22 @@
         <v>244</v>
       </c>
       <c r="B46" s="12" t="s">
-        <v>320</v>
+        <v>407</v>
       </c>
       <c r="C46" s="12" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D46" s="12" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E46" s="12" t="s">
         <v>80</v>
       </c>
       <c r="F46" s="12" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="G46" s="12" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="H46" s="12" t="s">
         <v>74</v>
@@ -4391,22 +4459,22 @@
         <v>245</v>
       </c>
       <c r="B47" s="12" t="s">
-        <v>320</v>
+        <v>407</v>
       </c>
       <c r="C47" s="12" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D47" s="12" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E47" s="12" t="s">
         <v>80</v>
       </c>
       <c r="F47" s="12" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="G47" s="12" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="H47" s="12" t="s">
         <v>74</v>
@@ -4430,22 +4498,22 @@
         <v>246</v>
       </c>
       <c r="B48" s="12" t="s">
-        <v>320</v>
+        <v>407</v>
       </c>
       <c r="C48" s="12" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D48" s="12" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E48" s="12" t="s">
         <v>108</v>
       </c>
       <c r="F48" s="12" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="G48" s="12" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="H48" s="12" t="s">
         <v>74</v>
@@ -4469,22 +4537,22 @@
         <v>259</v>
       </c>
       <c r="B49" s="12" t="s">
-        <v>320</v>
+        <v>407</v>
       </c>
       <c r="C49" s="12" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D49" s="12" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E49" s="12" t="s">
         <v>74</v>
       </c>
       <c r="F49" s="12" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G49" s="12" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="H49" s="12" t="s">
         <v>74</v>
@@ -4508,22 +4576,22 @@
         <v>234</v>
       </c>
       <c r="B50" s="12" t="s">
-        <v>320</v>
+        <v>407</v>
       </c>
       <c r="C50" s="12" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D50" s="12" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E50" s="12" t="s">
         <v>117</v>
       </c>
       <c r="F50" s="12" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="G50" s="12" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="H50" s="12" t="s">
         <v>78</v>
@@ -4547,13 +4615,13 @@
         <v>2</v>
       </c>
       <c r="B51" s="12" t="s">
-        <v>320</v>
+        <v>407</v>
       </c>
       <c r="C51" s="12" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D51" s="12" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E51" s="12" t="s">
         <v>117</v>
@@ -4562,7 +4630,7 @@
         <v>183</v>
       </c>
       <c r="G51" s="12" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="H51" s="12" t="s">
         <v>78</v>
@@ -4586,22 +4654,22 @@
         <v>265</v>
       </c>
       <c r="B52" s="12" t="s">
-        <v>320</v>
+        <v>407</v>
       </c>
       <c r="C52" s="12" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D52" s="12" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E52" s="12" t="s">
         <v>101</v>
       </c>
       <c r="F52" s="12" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="G52" s="12" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="H52" s="12" t="s">
         <v>78</v>
@@ -4625,22 +4693,22 @@
         <v>235</v>
       </c>
       <c r="B53" s="12" t="s">
-        <v>320</v>
+        <v>407</v>
       </c>
       <c r="C53" s="12" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D53" s="12" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E53" s="12" t="s">
         <v>97</v>
       </c>
       <c r="F53" s="12" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="G53" s="12" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="H53" s="12" t="s">
         <v>78</v>
@@ -4661,25 +4729,25 @@
     </row>
     <row r="54" spans="1:13">
       <c r="A54" s="12" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B54" s="12" t="s">
-        <v>320</v>
+        <v>407</v>
       </c>
       <c r="C54" s="12" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D54" s="12" t="s">
+        <v>329</v>
+      </c>
+      <c r="E54" s="12" t="s">
         <v>330</v>
       </c>
-      <c r="E54" s="12" t="s">
-        <v>331</v>
-      </c>
       <c r="F54" s="12" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="G54" s="12" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="H54" s="12" t="s">
         <v>78</v>
@@ -4703,22 +4771,22 @@
         <v>236</v>
       </c>
       <c r="B55" s="12" t="s">
-        <v>320</v>
+        <v>407</v>
       </c>
       <c r="C55" s="12" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D55" s="12" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E55" s="12" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="F55" s="12" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="G55" s="12" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="H55" s="12" t="s">
         <v>78</v>
@@ -4744,22 +4812,22 @@
         <v>237</v>
       </c>
       <c r="B56" s="12" t="s">
-        <v>320</v>
+        <v>407</v>
       </c>
       <c r="C56" s="12" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D56" s="12" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E56" s="12" t="s">
         <v>121</v>
       </c>
       <c r="F56" s="12" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="G56" s="12" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="H56" s="12" t="s">
         <v>78</v>
@@ -4783,22 +4851,22 @@
         <v>263</v>
       </c>
       <c r="B57" s="12" t="s">
-        <v>320</v>
+        <v>407</v>
       </c>
       <c r="C57" s="12" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D57" s="12" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E57" s="12" t="s">
         <v>103</v>
       </c>
       <c r="F57" s="12" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="G57" s="12" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="H57" s="12" t="s">
         <v>105</v>
@@ -4824,22 +4892,22 @@
         <v>5</v>
       </c>
       <c r="B58" s="12" t="s">
-        <v>320</v>
+        <v>407</v>
       </c>
       <c r="C58" s="12" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D58" s="12" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E58" s="12" t="s">
         <v>83</v>
       </c>
       <c r="F58" s="12" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="G58" s="12" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="H58" s="12" t="s">
         <v>78</v>
@@ -4863,13 +4931,13 @@
         <v>238</v>
       </c>
       <c r="B59" s="12" t="s">
-        <v>320</v>
+        <v>407</v>
       </c>
       <c r="C59" s="12" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D59" s="12" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E59" s="12" t="s">
         <v>83</v>
@@ -4878,7 +4946,7 @@
         <v>192</v>
       </c>
       <c r="G59" s="12" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="H59" s="12" t="s">
         <v>78</v>
@@ -4902,22 +4970,22 @@
         <v>239</v>
       </c>
       <c r="B60" s="12" t="s">
-        <v>320</v>
+        <v>407</v>
       </c>
       <c r="C60" s="12" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D60" s="12" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E60" s="12" t="s">
         <v>83</v>
       </c>
       <c r="F60" s="12" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="G60" s="12" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="H60" s="12" t="s">
         <v>78</v>
@@ -4941,13 +5009,13 @@
         <v>240</v>
       </c>
       <c r="B61" s="12" t="s">
-        <v>320</v>
+        <v>407</v>
       </c>
       <c r="C61" s="12" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D61" s="12" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E61" s="12" t="s">
         <v>83</v>
@@ -4956,7 +5024,7 @@
         <v>195</v>
       </c>
       <c r="G61" s="12" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="H61" s="12" t="s">
         <v>78</v>
@@ -4980,22 +5048,22 @@
         <v>241</v>
       </c>
       <c r="B62" s="12" t="s">
-        <v>320</v>
+        <v>407</v>
       </c>
       <c r="C62" s="12" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D62" s="12" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E62" s="12" t="s">
         <v>83</v>
       </c>
       <c r="F62" s="12" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="G62" s="12" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="H62" s="12" t="s">
         <v>78</v>
@@ -5019,22 +5087,22 @@
         <v>242</v>
       </c>
       <c r="B63" s="12" t="s">
-        <v>320</v>
+        <v>407</v>
       </c>
       <c r="C63" s="12" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D63" s="12" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E63" s="12" t="s">
         <v>90</v>
       </c>
       <c r="F63" s="12" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="G63" s="12" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="H63" s="12" t="s">
         <v>78</v>
@@ -5058,22 +5126,22 @@
         <v>247</v>
       </c>
       <c r="B64" s="12" t="s">
-        <v>320</v>
+        <v>407</v>
       </c>
       <c r="C64" s="12" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D64" s="12" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E64" s="12" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="F64" s="12" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="G64" s="12" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="H64" s="12" t="s">
         <v>74</v>
@@ -5097,22 +5165,22 @@
         <v>248</v>
       </c>
       <c r="B65" s="12" t="s">
-        <v>320</v>
+        <v>407</v>
       </c>
       <c r="C65" s="12" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D65" s="12" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E65" s="12" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="F65" s="12" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="G65" s="12" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="H65" s="12" t="s">
         <v>74</v>
@@ -5136,22 +5204,22 @@
         <v>249</v>
       </c>
       <c r="B66" s="12" t="s">
-        <v>320</v>
+        <v>407</v>
       </c>
       <c r="C66" s="12" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D66" s="12" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E66" s="12" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="F66" s="12" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="G66" s="12" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="H66" s="12" t="s">
         <v>74</v>
@@ -5175,17 +5243,17 @@
         <v>272</v>
       </c>
       <c r="B67" s="4" t="s">
+        <v>408</v>
+      </c>
+      <c r="C67" s="4" t="s">
+        <v>401</v>
+      </c>
+      <c r="D67" s="4" t="s">
         <v>320</v>
-      </c>
-      <c r="C67" s="4" t="s">
-        <v>402</v>
-      </c>
-      <c r="D67" s="4" t="s">
-        <v>321</v>
       </c>
       <c r="E67" s="4"/>
       <c r="F67" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="G67" s="4" t="s">
         <v>132</v>
@@ -5214,13 +5282,13 @@
         <v>278</v>
       </c>
       <c r="B68" s="4" t="s">
+        <v>408</v>
+      </c>
+      <c r="C68" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="D68" s="4" t="s">
         <v>320</v>
-      </c>
-      <c r="C68" s="3" t="s">
-        <v>402</v>
-      </c>
-      <c r="D68" s="4" t="s">
-        <v>321</v>
       </c>
       <c r="E68" s="4"/>
       <c r="F68" s="4" t="s">
@@ -5249,13 +5317,13 @@
         <v>279</v>
       </c>
       <c r="B69" s="4" t="s">
+        <v>408</v>
+      </c>
+      <c r="C69" s="4" t="s">
+        <v>401</v>
+      </c>
+      <c r="D69" s="4" t="s">
         <v>320</v>
-      </c>
-      <c r="C69" s="4" t="s">
-        <v>402</v>
-      </c>
-      <c r="D69" s="4" t="s">
-        <v>321</v>
       </c>
       <c r="E69" s="4"/>
       <c r="F69" s="4" t="s">
@@ -5284,13 +5352,13 @@
         <v>280</v>
       </c>
       <c r="B70" s="4" t="s">
+        <v>408</v>
+      </c>
+      <c r="C70" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="D70" s="4" t="s">
         <v>320</v>
-      </c>
-      <c r="C70" s="3" t="s">
-        <v>402</v>
-      </c>
-      <c r="D70" s="4" t="s">
-        <v>321</v>
       </c>
       <c r="E70" s="4"/>
       <c r="F70" s="4" t="s">
@@ -5319,13 +5387,13 @@
         <v>281</v>
       </c>
       <c r="B71" s="4" t="s">
+        <v>408</v>
+      </c>
+      <c r="C71" s="4" t="s">
+        <v>401</v>
+      </c>
+      <c r="D71" s="4" t="s">
         <v>320</v>
-      </c>
-      <c r="C71" s="4" t="s">
-        <v>402</v>
-      </c>
-      <c r="D71" s="4" t="s">
-        <v>321</v>
       </c>
       <c r="E71" s="4"/>
       <c r="F71" s="4" t="s">
@@ -5354,17 +5422,17 @@
         <v>273</v>
       </c>
       <c r="B72" s="4" t="s">
+        <v>408</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="D72" s="4" t="s">
         <v>320</v>
-      </c>
-      <c r="C72" s="3" t="s">
-        <v>402</v>
-      </c>
-      <c r="D72" s="4" t="s">
-        <v>321</v>
       </c>
       <c r="E72" s="4"/>
       <c r="F72" s="4" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="G72" s="4" t="s">
         <v>129</v>
@@ -5391,13 +5459,13 @@
         <v>283</v>
       </c>
       <c r="B73" s="4" t="s">
+        <v>408</v>
+      </c>
+      <c r="C73" s="4" t="s">
+        <v>401</v>
+      </c>
+      <c r="D73" s="4" t="s">
         <v>320</v>
-      </c>
-      <c r="C73" s="4" t="s">
-        <v>402</v>
-      </c>
-      <c r="D73" s="4" t="s">
-        <v>321</v>
       </c>
       <c r="E73" s="4"/>
       <c r="F73" s="4" t="s">
@@ -5426,13 +5494,13 @@
         <v>284</v>
       </c>
       <c r="B74" s="4" t="s">
+        <v>408</v>
+      </c>
+      <c r="C74" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="D74" s="4" t="s">
         <v>320</v>
-      </c>
-      <c r="C74" s="3" t="s">
-        <v>402</v>
-      </c>
-      <c r="D74" s="4" t="s">
-        <v>321</v>
       </c>
       <c r="E74" s="4"/>
       <c r="F74" s="4" t="s">
@@ -5461,13 +5529,13 @@
         <v>285</v>
       </c>
       <c r="B75" s="4" t="s">
+        <v>408</v>
+      </c>
+      <c r="C75" s="4" t="s">
+        <v>401</v>
+      </c>
+      <c r="D75" s="4" t="s">
         <v>320</v>
-      </c>
-      <c r="C75" s="4" t="s">
-        <v>402</v>
-      </c>
-      <c r="D75" s="4" t="s">
-        <v>321</v>
       </c>
       <c r="E75" s="4"/>
       <c r="F75" s="4" t="s">
@@ -5496,17 +5564,17 @@
         <v>274</v>
       </c>
       <c r="B76" s="4" t="s">
+        <v>408</v>
+      </c>
+      <c r="C76" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="D76" s="4" t="s">
         <v>320</v>
-      </c>
-      <c r="C76" s="3" t="s">
-        <v>402</v>
-      </c>
-      <c r="D76" s="4" t="s">
-        <v>321</v>
       </c>
       <c r="E76" s="4"/>
       <c r="F76" s="4" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="G76" s="4" t="s">
         <v>80</v>
@@ -5533,17 +5601,17 @@
         <v>275</v>
       </c>
       <c r="B77" s="4" t="s">
+        <v>408</v>
+      </c>
+      <c r="C77" s="4" t="s">
+        <v>401</v>
+      </c>
+      <c r="D77" s="4" t="s">
         <v>320</v>
-      </c>
-      <c r="C77" s="4" t="s">
-        <v>402</v>
-      </c>
-      <c r="D77" s="4" t="s">
-        <v>321</v>
       </c>
       <c r="E77" s="4"/>
       <c r="F77" s="4" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="G77" s="4" t="s">
         <v>80</v>
@@ -5570,13 +5638,13 @@
         <v>282</v>
       </c>
       <c r="B78" s="4" t="s">
+        <v>408</v>
+      </c>
+      <c r="C78" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="D78" s="4" t="s">
         <v>320</v>
-      </c>
-      <c r="C78" s="3" t="s">
-        <v>402</v>
-      </c>
-      <c r="D78" s="4" t="s">
-        <v>321</v>
       </c>
       <c r="E78" s="4"/>
       <c r="F78" s="4" t="s">
@@ -5605,17 +5673,17 @@
         <v>167</v>
       </c>
       <c r="B79" s="4" t="s">
+        <v>408</v>
+      </c>
+      <c r="C79" s="4" t="s">
+        <v>401</v>
+      </c>
+      <c r="D79" s="4" t="s">
         <v>320</v>
-      </c>
-      <c r="C79" s="4" t="s">
-        <v>402</v>
-      </c>
-      <c r="D79" s="4" t="s">
-        <v>321</v>
       </c>
       <c r="E79" s="4"/>
       <c r="F79" s="4" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="G79" s="4" t="s">
         <v>155</v>
@@ -5644,17 +5712,17 @@
         <v>276</v>
       </c>
       <c r="B80" s="4" t="s">
+        <v>408</v>
+      </c>
+      <c r="C80" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="D80" s="4" t="s">
         <v>320</v>
-      </c>
-      <c r="C80" s="3" t="s">
-        <v>402</v>
-      </c>
-      <c r="D80" s="4" t="s">
-        <v>321</v>
       </c>
       <c r="E80" s="4"/>
       <c r="F80" s="4" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="G80" s="4" t="s">
         <v>108</v>
@@ -5681,13 +5749,13 @@
         <v>302</v>
       </c>
       <c r="B81" s="4" t="s">
+        <v>408</v>
+      </c>
+      <c r="C81" s="4" t="s">
+        <v>401</v>
+      </c>
+      <c r="D81" s="4" t="s">
         <v>320</v>
-      </c>
-      <c r="C81" s="4" t="s">
-        <v>402</v>
-      </c>
-      <c r="D81" s="4" t="s">
-        <v>321</v>
       </c>
       <c r="E81" s="4"/>
       <c r="F81" s="4" t="s">
@@ -5716,17 +5784,17 @@
         <v>266</v>
       </c>
       <c r="B82" s="4" t="s">
+        <v>408</v>
+      </c>
+      <c r="C82" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="D82" s="4" t="s">
         <v>320</v>
-      </c>
-      <c r="C82" s="3" t="s">
-        <v>402</v>
-      </c>
-      <c r="D82" s="4" t="s">
-        <v>321</v>
       </c>
       <c r="E82" s="4"/>
       <c r="F82" s="4" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="G82" s="4" t="s">
         <v>142</v>
@@ -5753,17 +5821,17 @@
         <v>300</v>
       </c>
       <c r="B83" s="4" t="s">
+        <v>408</v>
+      </c>
+      <c r="C83" s="4" t="s">
+        <v>401</v>
+      </c>
+      <c r="D83" s="4" t="s">
         <v>320</v>
-      </c>
-      <c r="C83" s="4" t="s">
-        <v>402</v>
-      </c>
-      <c r="D83" s="4" t="s">
-        <v>321</v>
       </c>
       <c r="E83" s="4"/>
       <c r="F83" s="4" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="G83" s="4" t="s">
         <v>158</v>
@@ -5792,17 +5860,17 @@
         <v>267</v>
       </c>
       <c r="B84" s="4" t="s">
+        <v>408</v>
+      </c>
+      <c r="C84" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="D84" s="4" t="s">
         <v>320</v>
-      </c>
-      <c r="C84" s="3" t="s">
-        <v>402</v>
-      </c>
-      <c r="D84" s="4" t="s">
-        <v>321</v>
       </c>
       <c r="E84" s="4"/>
       <c r="F84" s="4" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="G84" s="4" t="s">
         <v>77</v>
@@ -5829,17 +5897,17 @@
         <v>297</v>
       </c>
       <c r="B85" s="4" t="s">
+        <v>408</v>
+      </c>
+      <c r="C85" s="4" t="s">
+        <v>401</v>
+      </c>
+      <c r="D85" s="4" t="s">
         <v>320</v>
-      </c>
-      <c r="C85" s="4" t="s">
-        <v>402</v>
-      </c>
-      <c r="D85" s="4" t="s">
-        <v>321</v>
       </c>
       <c r="E85" s="4"/>
       <c r="F85" s="4" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="G85" s="4" t="s">
         <v>77</v>
@@ -5866,17 +5934,17 @@
         <v>298</v>
       </c>
       <c r="B86" s="4" t="s">
+        <v>408</v>
+      </c>
+      <c r="C86" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="D86" s="4" t="s">
         <v>320</v>
-      </c>
-      <c r="C86" s="3" t="s">
-        <v>402</v>
-      </c>
-      <c r="D86" s="4" t="s">
-        <v>321</v>
       </c>
       <c r="E86" s="4"/>
       <c r="F86" s="4" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="G86" s="4" t="s">
         <v>77</v>
@@ -5905,13 +5973,13 @@
         <v>286</v>
       </c>
       <c r="B87" s="4" t="s">
+        <v>408</v>
+      </c>
+      <c r="C87" s="4" t="s">
+        <v>401</v>
+      </c>
+      <c r="D87" s="4" t="s">
         <v>320</v>
-      </c>
-      <c r="C87" s="4" t="s">
-        <v>402</v>
-      </c>
-      <c r="D87" s="4" t="s">
-        <v>321</v>
       </c>
       <c r="E87" s="4"/>
       <c r="F87" s="4" t="s">
@@ -5940,13 +6008,13 @@
         <v>287</v>
       </c>
       <c r="B88" s="4" t="s">
+        <v>408</v>
+      </c>
+      <c r="C88" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="D88" s="4" t="s">
         <v>320</v>
-      </c>
-      <c r="C88" s="3" t="s">
-        <v>402</v>
-      </c>
-      <c r="D88" s="4" t="s">
-        <v>321</v>
       </c>
       <c r="E88" s="4"/>
       <c r="F88" s="4" t="s">
@@ -5975,13 +6043,13 @@
         <v>288</v>
       </c>
       <c r="B89" s="4" t="s">
+        <v>408</v>
+      </c>
+      <c r="C89" s="4" t="s">
+        <v>401</v>
+      </c>
+      <c r="D89" s="4" t="s">
         <v>320</v>
-      </c>
-      <c r="C89" s="4" t="s">
-        <v>402</v>
-      </c>
-      <c r="D89" s="4" t="s">
-        <v>321</v>
       </c>
       <c r="E89" s="4"/>
       <c r="F89" s="4" t="s">
@@ -6010,13 +6078,13 @@
         <v>289</v>
       </c>
       <c r="B90" s="4" t="s">
+        <v>408</v>
+      </c>
+      <c r="C90" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="D90" s="4" t="s">
         <v>320</v>
-      </c>
-      <c r="C90" s="3" t="s">
-        <v>402</v>
-      </c>
-      <c r="D90" s="4" t="s">
-        <v>321</v>
       </c>
       <c r="E90" s="4"/>
       <c r="F90" s="4" t="s">
@@ -6045,13 +6113,13 @@
         <v>290</v>
       </c>
       <c r="B91" s="4" t="s">
+        <v>408</v>
+      </c>
+      <c r="C91" s="4" t="s">
+        <v>401</v>
+      </c>
+      <c r="D91" s="4" t="s">
         <v>320</v>
-      </c>
-      <c r="C91" s="4" t="s">
-        <v>402</v>
-      </c>
-      <c r="D91" s="4" t="s">
-        <v>321</v>
       </c>
       <c r="E91" s="4"/>
       <c r="F91" s="4" t="s">
@@ -6080,13 +6148,13 @@
         <v>291</v>
       </c>
       <c r="B92" s="4" t="s">
+        <v>408</v>
+      </c>
+      <c r="C92" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="D92" s="4" t="s">
         <v>320</v>
-      </c>
-      <c r="C92" s="3" t="s">
-        <v>402</v>
-      </c>
-      <c r="D92" s="4" t="s">
-        <v>321</v>
       </c>
       <c r="E92" s="4"/>
       <c r="F92" s="4" t="s">
@@ -6115,19 +6183,19 @@
         <v>305</v>
       </c>
       <c r="B93" s="4" t="s">
+        <v>408</v>
+      </c>
+      <c r="C93" s="4" t="s">
+        <v>401</v>
+      </c>
+      <c r="D93" s="4" t="s">
         <v>320</v>
       </c>
-      <c r="C93" s="4" t="s">
-        <v>402</v>
-      </c>
-      <c r="D93" s="4" t="s">
-        <v>321</v>
-      </c>
       <c r="E93" s="4" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="F93" s="4" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="G93" s="4" t="s">
         <v>77</v>
@@ -6154,17 +6222,17 @@
         <v>296</v>
       </c>
       <c r="B94" s="4" t="s">
+        <v>408</v>
+      </c>
+      <c r="C94" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="D94" s="4" t="s">
         <v>320</v>
-      </c>
-      <c r="C94" s="3" t="s">
-        <v>402</v>
-      </c>
-      <c r="D94" s="4" t="s">
-        <v>321</v>
       </c>
       <c r="E94" s="4"/>
       <c r="F94" s="4" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="G94" s="4" t="s">
         <v>104</v>
@@ -6193,17 +6261,17 @@
         <v>268</v>
       </c>
       <c r="B95" s="4" t="s">
+        <v>408</v>
+      </c>
+      <c r="C95" s="4" t="s">
+        <v>401</v>
+      </c>
+      <c r="D95" s="4" t="s">
         <v>320</v>
-      </c>
-      <c r="C95" s="4" t="s">
-        <v>402</v>
-      </c>
-      <c r="D95" s="4" t="s">
-        <v>321</v>
       </c>
       <c r="E95" s="4"/>
       <c r="F95" s="4" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="G95" s="4" t="s">
         <v>83</v>
@@ -6230,13 +6298,13 @@
         <v>269</v>
       </c>
       <c r="B96" s="4" t="s">
+        <v>408</v>
+      </c>
+      <c r="C96" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="D96" s="4" t="s">
         <v>320</v>
-      </c>
-      <c r="C96" s="3" t="s">
-        <v>402</v>
-      </c>
-      <c r="D96" s="4" t="s">
-        <v>321</v>
       </c>
       <c r="E96" s="4"/>
       <c r="F96" s="4" t="s">
@@ -6267,13 +6335,13 @@
         <v>270</v>
       </c>
       <c r="B97" s="4" t="s">
+        <v>408</v>
+      </c>
+      <c r="C97" s="4" t="s">
+        <v>401</v>
+      </c>
+      <c r="D97" s="4" t="s">
         <v>320</v>
-      </c>
-      <c r="C97" s="4" t="s">
-        <v>402</v>
-      </c>
-      <c r="D97" s="4" t="s">
-        <v>321</v>
       </c>
       <c r="E97" s="4"/>
       <c r="F97" s="4" t="s">
@@ -6304,17 +6372,17 @@
         <v>292</v>
       </c>
       <c r="B98" s="4" t="s">
+        <v>408</v>
+      </c>
+      <c r="C98" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="D98" s="4" t="s">
         <v>320</v>
-      </c>
-      <c r="C98" s="3" t="s">
-        <v>402</v>
-      </c>
-      <c r="D98" s="4" t="s">
-        <v>321</v>
       </c>
       <c r="E98" s="4"/>
       <c r="F98" s="4" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="G98" s="4" t="s">
         <v>83</v>
@@ -6339,17 +6407,17 @@
         <v>268</v>
       </c>
       <c r="B99" s="4" t="s">
+        <v>408</v>
+      </c>
+      <c r="C99" s="4" t="s">
+        <v>401</v>
+      </c>
+      <c r="D99" s="4" t="s">
         <v>320</v>
-      </c>
-      <c r="C99" s="4" t="s">
-        <v>402</v>
-      </c>
-      <c r="D99" s="4" t="s">
-        <v>321</v>
       </c>
       <c r="E99" s="4"/>
       <c r="F99" s="4" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="G99" s="4" t="s">
         <v>83</v>
@@ -6374,13 +6442,13 @@
         <v>293</v>
       </c>
       <c r="B100" s="4" t="s">
+        <v>408</v>
+      </c>
+      <c r="C100" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="D100" s="4" t="s">
         <v>320</v>
-      </c>
-      <c r="C100" s="3" t="s">
-        <v>402</v>
-      </c>
-      <c r="D100" s="4" t="s">
-        <v>321</v>
       </c>
       <c r="E100" s="4"/>
       <c r="F100" s="4" t="s">
@@ -6409,13 +6477,13 @@
         <v>294</v>
       </c>
       <c r="B101" s="4" t="s">
+        <v>408</v>
+      </c>
+      <c r="C101" s="4" t="s">
+        <v>401</v>
+      </c>
+      <c r="D101" s="4" t="s">
         <v>320</v>
-      </c>
-      <c r="C101" s="4" t="s">
-        <v>402</v>
-      </c>
-      <c r="D101" s="4" t="s">
-        <v>321</v>
       </c>
       <c r="E101" s="4"/>
       <c r="F101" s="4" t="s">
@@ -6444,13 +6512,13 @@
         <v>188</v>
       </c>
       <c r="B102" s="4" t="s">
+        <v>408</v>
+      </c>
+      <c r="C102" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="D102" s="4" t="s">
         <v>320</v>
-      </c>
-      <c r="C102" s="3" t="s">
-        <v>402</v>
-      </c>
-      <c r="D102" s="4" t="s">
-        <v>321</v>
       </c>
       <c r="E102" s="4"/>
       <c r="F102" s="4" t="s">
@@ -6479,13 +6547,13 @@
         <v>295</v>
       </c>
       <c r="B103" s="4" t="s">
+        <v>408</v>
+      </c>
+      <c r="C103" s="4" t="s">
+        <v>401</v>
+      </c>
+      <c r="D103" s="4" t="s">
         <v>320</v>
-      </c>
-      <c r="C103" s="4" t="s">
-        <v>402</v>
-      </c>
-      <c r="D103" s="4" t="s">
-        <v>321</v>
       </c>
       <c r="E103" s="4"/>
       <c r="F103" s="4" t="s">
@@ -6514,17 +6582,17 @@
         <v>271</v>
       </c>
       <c r="B104" s="4" t="s">
+        <v>408</v>
+      </c>
+      <c r="C104" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="D104" s="4" t="s">
         <v>320</v>
-      </c>
-      <c r="C104" s="3" t="s">
-        <v>402</v>
-      </c>
-      <c r="D104" s="4" t="s">
-        <v>321</v>
       </c>
       <c r="E104" s="4"/>
       <c r="F104" s="4" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="G104" s="4" t="s">
         <v>90</v>
@@ -6551,13 +6619,13 @@
         <v>271</v>
       </c>
       <c r="B105" s="4" t="s">
+        <v>408</v>
+      </c>
+      <c r="C105" s="4" t="s">
+        <v>401</v>
+      </c>
+      <c r="D105" s="4" t="s">
         <v>320</v>
-      </c>
-      <c r="C105" s="4" t="s">
-        <v>402</v>
-      </c>
-      <c r="D105" s="4" t="s">
-        <v>321</v>
       </c>
       <c r="E105" s="4"/>
       <c r="F105" s="4" t="s">
@@ -6586,17 +6654,17 @@
         <v>277</v>
       </c>
       <c r="B106" s="4" t="s">
+        <v>408</v>
+      </c>
+      <c r="C106" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="D106" s="4" t="s">
         <v>320</v>
-      </c>
-      <c r="C106" s="3" t="s">
-        <v>402</v>
-      </c>
-      <c r="D106" s="4" t="s">
-        <v>321</v>
       </c>
       <c r="E106" s="4"/>
       <c r="F106" s="4" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="G106" s="4" t="s">
         <v>93</v>
@@ -6623,17 +6691,17 @@
         <v>299</v>
       </c>
       <c r="B107" s="4" t="s">
+        <v>408</v>
+      </c>
+      <c r="C107" s="4" t="s">
+        <v>401</v>
+      </c>
+      <c r="D107" s="4" t="s">
         <v>320</v>
-      </c>
-      <c r="C107" s="4" t="s">
-        <v>402</v>
-      </c>
-      <c r="D107" s="4" t="s">
-        <v>321</v>
       </c>
       <c r="E107" s="4"/>
       <c r="F107" s="4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="G107" s="4" t="s">
         <v>93</v>
@@ -6660,13 +6728,13 @@
         <v>301</v>
       </c>
       <c r="B108" s="4" t="s">
+        <v>408</v>
+      </c>
+      <c r="C108" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="D108" s="4" t="s">
         <v>320</v>
-      </c>
-      <c r="C108" s="3" t="s">
-        <v>402</v>
-      </c>
-      <c r="D108" s="4" t="s">
-        <v>321</v>
       </c>
       <c r="E108" s="4"/>
       <c r="F108" s="4" t="s">
@@ -6695,19 +6763,19 @@
         <v>217</v>
       </c>
       <c r="B109" s="5" t="s">
-        <v>320</v>
+        <v>407</v>
       </c>
       <c r="C109" s="5" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D109" s="7" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="E109" s="5" t="s">
         <v>155</v>
       </c>
       <c r="F109" s="5" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="G109" s="5" t="s">
         <v>155</v>
@@ -6736,19 +6804,19 @@
         <v>176</v>
       </c>
       <c r="B110" s="5" t="s">
-        <v>320</v>
+        <v>407</v>
       </c>
       <c r="C110" s="5" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D110" s="7" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="E110" s="5" t="s">
         <v>158</v>
       </c>
       <c r="F110" s="5" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="G110" s="5" t="s">
         <v>158</v>

</xml_diff>

<commit_message>
Added 'existing member only' option to alignment import
</commit_message>
<xml_diff>
--- a/tabular/ifnl-side-data.xlsx
+++ b/tabular/ifnl-side-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/host/IFNL-Evolution/tabular/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C2D8795-1F28-1F4F-A1C0-FDB289475FE7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8AC14A8-F11A-B447-B26E-900DC95DA104}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4980" yWindow="460" windowWidth="23480" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2888,8 +2888,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="I42" sqref="A1:P127"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="H112" sqref="H112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>

<commit_message>
Refine phylogeny build and annotation export
</commit_message>
<xml_diff>
--- a/tabular/ifnl-side-data.xlsx
+++ b/tabular/ifnl-side-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/host/IFNL-Evolution/tabular/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CEFB389-80EB-A34B-B19C-8A4D6D9E3282}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{540C6AE5-B0EA-0A4A-B381-7B95CF46F912}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3000" yWindow="460" windowWidth="23480" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3273,8 +3273,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P204"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K185" workbookViewId="0">
-      <selection activeCell="P204" sqref="A1:P204"/>
+    <sheetView tabSelected="1" topLeftCell="A81" workbookViewId="0">
+      <selection activeCell="A185" sqref="A185"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>

<commit_message>
Updated trees to include species taxonomy
</commit_message>
<xml_diff>
--- a/tabular/ifnl-side-data.xlsx
+++ b/tabular/ifnl-side-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/host/IFNL-Evolution/tabular/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B3B5398-6DA3-1D4B-A799-7369594C2711}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ACC2B9C-780D-E242-B6D5-39D8E0D299D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1636,9 +1636,6 @@
     <t>Superorder</t>
   </si>
   <si>
-    <t>Order</t>
-  </si>
-  <si>
     <t>Family</t>
   </si>
   <si>
@@ -1796,6 +1793,9 @@
   </si>
   <si>
     <t>Terrapene</t>
+  </si>
+  <si>
+    <t>Species_order</t>
   </si>
 </sst>
 </file>
@@ -3502,7 +3502,7 @@
   <dimension ref="A1:Q204"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="Q1" sqref="A1:Q1048576"/>
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3563,13 +3563,13 @@
         <v>535</v>
       </c>
       <c r="M1" s="1" t="s">
+        <v>589</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>536</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>537</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>538</v>
       </c>
       <c r="P1" s="37" t="s">
         <v>360</v>
@@ -4161,7 +4161,7 @@
         <v>100</v>
       </c>
       <c r="O15" s="3" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="P15" s="38"/>
       <c r="Q15" s="38"/>
@@ -4201,10 +4201,10 @@
         <v>92</v>
       </c>
       <c r="N16" s="3" t="s">
+        <v>539</v>
+      </c>
+      <c r="O16" s="3" t="s">
         <v>540</v>
-      </c>
-      <c r="O16" s="3" t="s">
-        <v>541</v>
       </c>
       <c r="P16" s="38"/>
       <c r="Q16" s="38"/>
@@ -4285,10 +4285,10 @@
         <v>92</v>
       </c>
       <c r="N18" s="10" t="s">
+        <v>541</v>
+      </c>
+      <c r="O18" s="10" t="s">
         <v>542</v>
-      </c>
-      <c r="O18" s="10" t="s">
-        <v>543</v>
       </c>
       <c r="P18" s="10"/>
       <c r="Q18" s="10"/>
@@ -4328,10 +4328,10 @@
         <v>131</v>
       </c>
       <c r="N19" s="3" t="s">
+        <v>543</v>
+      </c>
+      <c r="O19" s="3" t="s">
         <v>544</v>
-      </c>
-      <c r="O19" s="3" t="s">
-        <v>545</v>
       </c>
       <c r="P19" s="38"/>
       <c r="Q19" s="38"/>
@@ -4374,7 +4374,7 @@
         <v>78</v>
       </c>
       <c r="O20" s="3" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="P20" s="38"/>
       <c r="Q20" s="38"/>
@@ -5097,7 +5097,7 @@
         <v>78</v>
       </c>
       <c r="O37" s="3" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="P37" s="38"/>
       <c r="Q37" s="38"/>
@@ -5982,7 +5982,7 @@
         <v>100</v>
       </c>
       <c r="O58" s="3" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="P58" s="38"/>
       <c r="Q58" s="38"/>
@@ -6025,7 +6025,7 @@
         <v>94</v>
       </c>
       <c r="O59" s="3" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="P59" s="38"/>
       <c r="Q59" s="38"/>
@@ -6279,7 +6279,7 @@
         <v>130</v>
       </c>
       <c r="O65" s="3" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="P65" s="38"/>
       <c r="Q65" s="38"/>
@@ -6405,16 +6405,16 @@
       <c r="J68" s="35"/>
       <c r="K68" s="35"/>
       <c r="L68" s="35" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="M68" s="35" t="s">
         <v>419</v>
       </c>
       <c r="N68" s="35" t="s">
+        <v>551</v>
+      </c>
+      <c r="O68" s="35" t="s">
         <v>552</v>
-      </c>
-      <c r="O68" s="35" t="s">
-        <v>553</v>
       </c>
       <c r="P68" s="40"/>
       <c r="Q68" s="40"/>
@@ -6446,16 +6446,16 @@
       <c r="J69" s="35"/>
       <c r="K69" s="35"/>
       <c r="L69" s="35" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="M69" s="35" t="s">
         <v>419</v>
       </c>
       <c r="N69" s="35" t="s">
+        <v>553</v>
+      </c>
+      <c r="O69" s="35" t="s">
         <v>554</v>
-      </c>
-      <c r="O69" s="35" t="s">
-        <v>555</v>
       </c>
       <c r="P69" s="40"/>
       <c r="Q69" s="40"/>
@@ -6490,10 +6490,10 @@
         <v>92</v>
       </c>
       <c r="M70" s="30" t="s">
+        <v>555</v>
+      </c>
+      <c r="N70" s="30" t="s">
         <v>556</v>
-      </c>
-      <c r="N70" s="30" t="s">
-        <v>557</v>
       </c>
       <c r="O70" s="30" t="s">
         <v>336</v>
@@ -6533,10 +6533,10 @@
         <v>92</v>
       </c>
       <c r="M71" s="7" t="s">
+        <v>555</v>
+      </c>
+      <c r="N71" s="7" t="s">
         <v>556</v>
-      </c>
-      <c r="N71" s="7" t="s">
-        <v>557</v>
       </c>
       <c r="O71" s="7" t="s">
         <v>336</v>
@@ -6573,16 +6573,16 @@
       <c r="J72" s="9"/>
       <c r="K72" s="12"/>
       <c r="L72" s="9" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="M72" s="9" t="s">
         <v>335</v>
       </c>
       <c r="N72" s="9" t="s">
+        <v>558</v>
+      </c>
+      <c r="O72" s="9" t="s">
         <v>559</v>
-      </c>
-      <c r="O72" s="9" t="s">
-        <v>560</v>
       </c>
       <c r="P72" s="43"/>
       <c r="Q72" s="43"/>
@@ -6616,16 +6616,16 @@
       <c r="J73" s="8"/>
       <c r="K73" s="14"/>
       <c r="L73" s="8" t="s">
+        <v>560</v>
+      </c>
+      <c r="M73" s="8" t="s">
         <v>561</v>
       </c>
-      <c r="M73" s="8" t="s">
+      <c r="N73" s="8" t="s">
         <v>562</v>
       </c>
-      <c r="N73" s="8" t="s">
+      <c r="O73" s="8" t="s">
         <v>563</v>
-      </c>
-      <c r="O73" s="8" t="s">
-        <v>564</v>
       </c>
       <c r="P73" s="44"/>
       <c r="Q73" s="44"/>
@@ -6657,16 +6657,16 @@
       <c r="J74" s="8"/>
       <c r="K74" s="14"/>
       <c r="L74" s="8" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="M74" s="8" t="s">
+        <v>564</v>
+      </c>
+      <c r="N74" s="8" t="s">
         <v>565</v>
       </c>
-      <c r="N74" s="8" t="s">
+      <c r="O74" s="8" t="s">
         <v>566</v>
-      </c>
-      <c r="O74" s="8" t="s">
-        <v>567</v>
       </c>
       <c r="P74" s="44"/>
       <c r="Q74" s="44"/>
@@ -6698,16 +6698,16 @@
       <c r="J75" s="8"/>
       <c r="K75" s="14"/>
       <c r="L75" s="8" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="M75" s="8" t="s">
+        <v>567</v>
+      </c>
+      <c r="N75" s="8" t="s">
         <v>568</v>
       </c>
-      <c r="N75" s="8" t="s">
+      <c r="O75" s="8" t="s">
         <v>569</v>
-      </c>
-      <c r="O75" s="8" t="s">
-        <v>570</v>
       </c>
       <c r="P75" s="44"/>
       <c r="Q75" s="44"/>
@@ -6884,10 +6884,10 @@
         <v>131</v>
       </c>
       <c r="N79" s="4" t="s">
+        <v>570</v>
+      </c>
+      <c r="O79" s="4" t="s">
         <v>571</v>
-      </c>
-      <c r="O79" s="4" t="s">
-        <v>572</v>
       </c>
       <c r="P79" s="4"/>
       <c r="Q79" s="4"/>
@@ -6929,10 +6929,10 @@
         <v>131</v>
       </c>
       <c r="N80" s="4" t="s">
+        <v>570</v>
+      </c>
+      <c r="O80" s="4" t="s">
         <v>571</v>
-      </c>
-      <c r="O80" s="4" t="s">
-        <v>572</v>
       </c>
       <c r="P80" s="4"/>
       <c r="Q80" s="4"/>
@@ -6948,7 +6948,7 @@
         <v>309</v>
       </c>
       <c r="D81" s="4" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="E81" s="4"/>
       <c r="F81" s="4" t="s">
@@ -7105,10 +7105,10 @@
         <v>92</v>
       </c>
       <c r="N84" s="4" t="s">
+        <v>539</v>
+      </c>
+      <c r="O84" s="4" t="s">
         <v>540</v>
-      </c>
-      <c r="O84" s="4" t="s">
-        <v>541</v>
       </c>
       <c r="P84" s="4"/>
       <c r="Q84" s="4"/>
@@ -7153,7 +7153,7 @@
         <v>100</v>
       </c>
       <c r="O85" s="4" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="P85" s="4"/>
       <c r="Q85" s="4"/>
@@ -7330,10 +7330,10 @@
         <v>92</v>
       </c>
       <c r="N89" s="4" t="s">
+        <v>541</v>
+      </c>
+      <c r="O89" s="4" t="s">
         <v>542</v>
-      </c>
-      <c r="O89" s="4" t="s">
-        <v>543</v>
       </c>
       <c r="P89" s="4"/>
       <c r="Q89" s="4"/>
@@ -7373,10 +7373,10 @@
         <v>92</v>
       </c>
       <c r="N90" s="4" t="s">
+        <v>541</v>
+      </c>
+      <c r="O90" s="4" t="s">
         <v>542</v>
-      </c>
-      <c r="O90" s="4" t="s">
-        <v>543</v>
       </c>
       <c r="P90" s="4"/>
       <c r="Q90" s="4"/>
@@ -7828,7 +7828,7 @@
         <v>78</v>
       </c>
       <c r="O100" s="4" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="P100" s="4"/>
       <c r="Q100" s="4"/>
@@ -7870,7 +7870,7 @@
         <v>82</v>
       </c>
       <c r="N101" s="4" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="O101" s="4" t="s">
         <v>394</v>
@@ -8413,7 +8413,7 @@
         <v>94</v>
       </c>
       <c r="O113" s="4" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="P113" s="4"/>
       <c r="Q113" s="4"/>
@@ -9461,7 +9461,7 @@
         <v>125</v>
       </c>
       <c r="O135" s="10" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="P135" s="10"/>
       <c r="Q135" s="10"/>
@@ -9506,7 +9506,7 @@
         <v>125</v>
       </c>
       <c r="O136" s="10" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="P136" s="10"/>
       <c r="Q136" s="10"/>
@@ -9522,7 +9522,7 @@
         <v>309</v>
       </c>
       <c r="D137" s="10" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="E137" s="10"/>
       <c r="F137" s="10" t="s">
@@ -9830,10 +9830,10 @@
         <v>92</v>
       </c>
       <c r="N143" s="10" t="s">
+        <v>541</v>
+      </c>
+      <c r="O143" s="10" t="s">
         <v>542</v>
-      </c>
-      <c r="O143" s="10" t="s">
-        <v>543</v>
       </c>
       <c r="P143" s="10"/>
       <c r="Q143" s="10"/>
@@ -9874,13 +9874,13 @@
         <v>104</v>
       </c>
       <c r="M144" s="10" t="s">
+        <v>576</v>
+      </c>
+      <c r="N144" s="10" t="s">
         <v>577</v>
       </c>
-      <c r="N144" s="10" t="s">
+      <c r="O144" s="10" t="s">
         <v>578</v>
-      </c>
-      <c r="O144" s="10" t="s">
-        <v>579</v>
       </c>
       <c r="P144" s="10"/>
       <c r="Q144" s="10"/>
@@ -9927,7 +9927,7 @@
         <v>78</v>
       </c>
       <c r="O145" s="10" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="P145" s="10"/>
       <c r="Q145" s="10"/>
@@ -10491,7 +10491,7 @@
         <v>78</v>
       </c>
       <c r="O157" s="10" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="P157" s="10"/>
       <c r="Q157" s="10"/>
@@ -10536,7 +10536,7 @@
         <v>78</v>
       </c>
       <c r="O158" s="10" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="P158" s="10"/>
       <c r="Q158" s="10"/>
@@ -10581,7 +10581,7 @@
         <v>78</v>
       </c>
       <c r="O159" s="10" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="P159" s="10"/>
       <c r="Q159" s="10"/>
@@ -10622,13 +10622,13 @@
         <v>92</v>
       </c>
       <c r="M160" s="10" t="s">
+        <v>579</v>
+      </c>
+      <c r="N160" s="10" t="s">
         <v>580</v>
       </c>
-      <c r="N160" s="10" t="s">
+      <c r="O160" s="10" t="s">
         <v>581</v>
-      </c>
-      <c r="O160" s="10" t="s">
-        <v>582</v>
       </c>
       <c r="P160" s="10"/>
       <c r="Q160" s="10"/>
@@ -10670,7 +10670,7 @@
         <v>82</v>
       </c>
       <c r="N161" s="10" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="O161" s="10" t="s">
         <v>394</v>
@@ -10715,7 +10715,7 @@
         <v>82</v>
       </c>
       <c r="N162" s="10" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="O162" s="10" t="s">
         <v>394</v>
@@ -10760,7 +10760,7 @@
         <v>82</v>
       </c>
       <c r="N163" s="10" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="O163" s="10" t="s">
         <v>394</v>
@@ -10807,7 +10807,7 @@
         <v>82</v>
       </c>
       <c r="N164" s="10" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="O164" s="10" t="s">
         <v>394</v>
@@ -10854,7 +10854,7 @@
         <v>82</v>
       </c>
       <c r="N165" s="10" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="O165" s="10" t="s">
         <v>394</v>
@@ -11926,7 +11926,7 @@
         <v>94</v>
       </c>
       <c r="O188" s="10" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="P188" s="10"/>
       <c r="Q188" s="10"/>
@@ -11971,7 +11971,7 @@
         <v>94</v>
       </c>
       <c r="O189" s="10" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="P189" s="10"/>
       <c r="Q189" s="10"/>
@@ -12018,7 +12018,7 @@
         <v>94</v>
       </c>
       <c r="O190" s="10" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="P190" s="10"/>
       <c r="Q190" s="10"/>
@@ -12065,7 +12065,7 @@
         <v>94</v>
       </c>
       <c r="O191" s="10" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="P191" s="10"/>
       <c r="Q191" s="10"/>
@@ -12247,13 +12247,13 @@
         <v>92</v>
       </c>
       <c r="M195" s="10" t="s">
+        <v>582</v>
+      </c>
+      <c r="N195" s="10" t="s">
         <v>583</v>
       </c>
-      <c r="N195" s="10" t="s">
+      <c r="O195" s="10" t="s">
         <v>584</v>
-      </c>
-      <c r="O195" s="10" t="s">
-        <v>585</v>
       </c>
       <c r="P195" s="10"/>
       <c r="Q195" s="10"/>
@@ -12618,10 +12618,10 @@
         <v>337</v>
       </c>
       <c r="N203" s="7" t="s">
+        <v>585</v>
+      </c>
+      <c r="O203" s="7" t="s">
         <v>586</v>
-      </c>
-      <c r="O203" s="7" t="s">
-        <v>587</v>
       </c>
       <c r="P203" s="41"/>
       <c r="Q203" s="41"/>
@@ -12659,10 +12659,10 @@
         <v>337</v>
       </c>
       <c r="N204" s="7" t="s">
+        <v>587</v>
+      </c>
+      <c r="O204" s="7" t="s">
         <v>588</v>
-      </c>
-      <c r="O204" s="7" t="s">
-        <v>589</v>
       </c>
       <c r="P204" s="41"/>
       <c r="Q204" s="41"/>

</xml_diff>